<commit_message>
changed TestData for Datadriven Login Changed ExtentReport Changed Common step def regading testdata code changed in utilities as well sa for test data reading code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/dsAlgoTestData.xlsx
+++ b/src/test/resources/TestData/dsAlgoTestData.xlsx
@@ -3,20 +3,33 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="PythonArray" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="PythonArray" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="UL5Lqr9PbOgeey+9JMNi0TcbUAsQXs6ahhR0Sd+HNsY="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="xiQ+14SZppxkpB3hF2CpN5YgPYHGoCsLamLy7CqNZLI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Group1@dslgo</t>
+  </si>
+  <si>
+    <t>dsalgo2024</t>
+  </si>
   <si>
     <t>PythonCode for Array in tryedior arrays in python</t>
   </si>
@@ -58,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -68,14 +81,30 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,12 +113,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -101,6 +136,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -301,6 +340,37 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -314,59 +384,59 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+      <c r="A3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
+      <c r="A6" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
+      <c r="A7" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
+      <c r="A8" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
+      <c r="A9" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
+      <c r="A10" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>